<commit_message>
Fixed sample portfolio 1 delta matrix
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Group ALM\Ville\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ilmari/Documents/OR semma/entropy-poolin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A6F35A0-90F8-4284-AC72-5149B6A09F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D950C2C9-513F-9C43-AF0B-A8EE2B07A2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-390" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{F9C29C47-E65C-40D9-8125-D2F4D60475BD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" activeTab="1" xr2:uid="{F9C29C47-E65C-40D9-8125-D2F4D60475BD}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="3" r:id="rId1"/>
@@ -19,8 +19,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'DATA BROWSER'!$D$1:$D$252</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'DATA BROWSER'!#REF!</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'DATA BROWSER'!$D$1:$D$252</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -312,7 +310,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -417,7 +415,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -426,6 +424,95 @@
   </cellStyles>
   <dxfs count="45">
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -434,6 +521,29 @@
       </fill>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -766,22 +876,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -790,108 +884,12 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1536,8 +1534,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="1447800"/>
-              <a:ext cx="6153150" cy="3076575"/>
+              <a:off x="0" y="1422400"/>
+              <a:ext cx="6146800" cy="3022600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1556,7 +1554,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="fi-FI" sz="1100"/>
+                <a:rPr lang="en-GB" sz="1100"/>
                 <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
@@ -1571,60 +1569,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A84C2F7B-0267-4AE8-B2F1-2249AF7E1605}" name="Chi" displayName="Chi" ref="A1:AJ253" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A84C2F7B-0267-4AE8-B2F1-2249AF7E1605}" name="Chi" displayName="Chi" ref="A1:AJ253" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <tableColumns count="36">
-    <tableColumn id="1" xr3:uid="{CD2FB1E1-FE78-4156-BC9E-63CEDA3E4875}" name="Global Equities" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{A02B6FB9-8285-429C-A5CC-F29BF66F2A79}" name="DM Equities" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{94C4C328-15A5-4A56-BCCF-A53780FEF28F}" name="EM Equities" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{0FCF531F-0CBE-4CBF-AB2B-DAC3BE704180}" name="European Equities" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{F9C8619E-F77F-4977-8CA5-06AB4EAEAB26}" name="US Equities" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{39DC7D8D-CA36-4990-95A1-DC0C6412792F}" name="EUR Money Markets" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{90DF8663-8322-46BE-B390-FD393C54F2A3}" name="EUR Government Bonds" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{A91B4CB4-4D1C-4C3F-B1F3-89D67D75766F}" name="EUR Covered Bonds" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{80827C12-5D88-4C5B-A558-F98F705837AB}" name="EUR Investment Grade Corporate Bonds" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{D3675369-4FE4-4651-A577-4117B2700180}" name="European High Yield Corporate Bonds" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{5889AC42-4DB6-4FBB-92FB-F559D01BE452}" name="EMD Hard Currency" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{5BC385A4-1545-44FA-82EC-6E200749EA82}" name="Hedge Funds" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{FC7AF93B-AB9A-4758-8240-ABC50598907B}" name="Listed Private Equity" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{E34D9AFC-2075-4A7B-9B24-42EFDD48F888}" name="1Y EUR SWAP" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{5AEC84DC-F474-4F56-B357-362BD17DAEEE}" name="2Y EUR SWAP" dataDxfId="23"/>
-    <tableColumn id="16" xr3:uid="{8CF9F4DA-5556-467C-B676-2B51CC7AED23}" name="3Y EUR SWAP" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{23D73306-B2CB-40CA-ACA4-592AA360F5EE}" name="5Y EUR SWAP" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{3F01D429-279E-46D2-9C3E-A2B687639774}" name="7Y EUR SWAP" dataDxfId="20"/>
-    <tableColumn id="19" xr3:uid="{09894B42-740E-4A1A-9123-BF597F4CA8FC}" name="10Y EUR SWAP" dataDxfId="19"/>
-    <tableColumn id="20" xr3:uid="{6CBF5233-1D2C-4E1D-AEBD-5D0EA999B456}" name="15Y EUR SWAP" dataDxfId="18"/>
-    <tableColumn id="21" xr3:uid="{85F083D1-0FBC-4520-8115-89D7D3FE7237}" name="20Y EUR SWAP" dataDxfId="17"/>
-    <tableColumn id="22" xr3:uid="{51CCDE5D-06DE-497B-87DC-B5E26FB08472}" name="30Y EUR SWAP" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{A9025FB0-8CF5-49F3-8ECF-0C43078F32A1}" name="50Y EUR SWAP" dataDxfId="15"/>
-    <tableColumn id="24" xr3:uid="{0F535407-A2AD-4EBF-BFF1-0EC8EA996DA9}" name="EURUSD" dataDxfId="14"/>
-    <tableColumn id="25" xr3:uid="{EC3E41BE-2E18-4947-8830-4E9EBB30C0E9}" name="US 10-Year Treasury Yield" dataDxfId="13"/>
-    <tableColumn id="26" xr3:uid="{7007A639-1F35-4A36-8BD2-0ACF9AC1E91E}" name="Germany 10-Year Government Bond Yield" dataDxfId="12"/>
-    <tableColumn id="27" xr3:uid="{0E480D66-5661-41A8-9CA3-BA7974728C49}" name="iVol US Equities" dataDxfId="11"/>
-    <tableColumn id="28" xr3:uid="{C25B1846-475B-47D2-BF1C-6E0DA8B703B5}" name="iVol European Equities" dataDxfId="10"/>
-    <tableColumn id="29" xr3:uid="{87F6798F-4B20-41E4-B769-4276FC113D1F}" name="FED Balance Sheet Total" dataDxfId="9"/>
-    <tableColumn id="30" xr3:uid="{E76EC533-1CFA-47A5-ADF8-7038464A2F60}" name="Eurosystem Balance Sheet Total" dataDxfId="8"/>
-    <tableColumn id="31" xr3:uid="{7791EA87-EAFC-4D2D-8036-CF6616A55DDB}" name="US Core Inflation" dataDxfId="7"/>
-    <tableColumn id="32" xr3:uid="{84A946B2-BC3D-4910-A0B8-DBC39C164652}" name="US Unemployment" dataDxfId="6"/>
-    <tableColumn id="33" xr3:uid="{95419E23-D2CF-4363-BBB2-F3CF2AF2B5EF}" name="US Manufacturing PMI" dataDxfId="5"/>
-    <tableColumn id="34" xr3:uid="{227E5F86-CFBB-4C03-BEF4-03EF7FE57B36}" name="US Services PMI" dataDxfId="4"/>
-    <tableColumn id="35" xr3:uid="{756F9EC1-6A7F-4644-822F-C0FB7871DB43}" name="Eurozone Core Inflation" dataDxfId="3"/>
-    <tableColumn id="36" xr3:uid="{4CC0EE89-317B-47F2-A10D-F3CDBFBD5D1C}" name="Eurozone Unemployment" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CD2FB1E1-FE78-4156-BC9E-63CEDA3E4875}" name="Global Equities" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{A02B6FB9-8285-429C-A5CC-F29BF66F2A79}" name="DM Equities" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{94C4C328-15A5-4A56-BCCF-A53780FEF28F}" name="EM Equities" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{0FCF531F-0CBE-4CBF-AB2B-DAC3BE704180}" name="European Equities" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{F9C8619E-F77F-4977-8CA5-06AB4EAEAB26}" name="US Equities" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{39DC7D8D-CA36-4990-95A1-DC0C6412792F}" name="EUR Money Markets" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{90DF8663-8322-46BE-B390-FD393C54F2A3}" name="EUR Government Bonds" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{A91B4CB4-4D1C-4C3F-B1F3-89D67D75766F}" name="EUR Covered Bonds" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{80827C12-5D88-4C5B-A558-F98F705837AB}" name="EUR Investment Grade Corporate Bonds" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{D3675369-4FE4-4651-A577-4117B2700180}" name="European High Yield Corporate Bonds" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{5889AC42-4DB6-4FBB-92FB-F559D01BE452}" name="EMD Hard Currency" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{5BC385A4-1545-44FA-82EC-6E200749EA82}" name="Hedge Funds" dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{FC7AF93B-AB9A-4758-8240-ABC50598907B}" name="Listed Private Equity" dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{E34D9AFC-2075-4A7B-9B24-42EFDD48F888}" name="1Y EUR SWAP" dataDxfId="29"/>
+    <tableColumn id="15" xr3:uid="{5AEC84DC-F474-4F56-B357-362BD17DAEEE}" name="2Y EUR SWAP" dataDxfId="28"/>
+    <tableColumn id="16" xr3:uid="{8CF9F4DA-5556-467C-B676-2B51CC7AED23}" name="3Y EUR SWAP" dataDxfId="27"/>
+    <tableColumn id="17" xr3:uid="{23D73306-B2CB-40CA-ACA4-592AA360F5EE}" name="5Y EUR SWAP" dataDxfId="26"/>
+    <tableColumn id="18" xr3:uid="{3F01D429-279E-46D2-9C3E-A2B687639774}" name="7Y EUR SWAP" dataDxfId="25"/>
+    <tableColumn id="19" xr3:uid="{09894B42-740E-4A1A-9123-BF597F4CA8FC}" name="10Y EUR SWAP" dataDxfId="24"/>
+    <tableColumn id="20" xr3:uid="{6CBF5233-1D2C-4E1D-AEBD-5D0EA999B456}" name="15Y EUR SWAP" dataDxfId="23"/>
+    <tableColumn id="21" xr3:uid="{85F083D1-0FBC-4520-8115-89D7D3FE7237}" name="20Y EUR SWAP" dataDxfId="22"/>
+    <tableColumn id="22" xr3:uid="{51CCDE5D-06DE-497B-87DC-B5E26FB08472}" name="30Y EUR SWAP" dataDxfId="21"/>
+    <tableColumn id="23" xr3:uid="{A9025FB0-8CF5-49F3-8ECF-0C43078F32A1}" name="50Y EUR SWAP" dataDxfId="20"/>
+    <tableColumn id="24" xr3:uid="{0F535407-A2AD-4EBF-BFF1-0EC8EA996DA9}" name="EURUSD" dataDxfId="19"/>
+    <tableColumn id="25" xr3:uid="{EC3E41BE-2E18-4947-8830-4E9EBB30C0E9}" name="US 10-Year Treasury Yield" dataDxfId="18"/>
+    <tableColumn id="26" xr3:uid="{7007A639-1F35-4A36-8BD2-0ACF9AC1E91E}" name="Germany 10-Year Government Bond Yield" dataDxfId="17"/>
+    <tableColumn id="27" xr3:uid="{0E480D66-5661-41A8-9CA3-BA7974728C49}" name="iVol US Equities" dataDxfId="16"/>
+    <tableColumn id="28" xr3:uid="{C25B1846-475B-47D2-BF1C-6E0DA8B703B5}" name="iVol European Equities" dataDxfId="15"/>
+    <tableColumn id="29" xr3:uid="{87F6798F-4B20-41E4-B769-4276FC113D1F}" name="FED Balance Sheet Total" dataDxfId="14"/>
+    <tableColumn id="30" xr3:uid="{E76EC533-1CFA-47A5-ADF8-7038464A2F60}" name="Eurosystem Balance Sheet Total" dataDxfId="13"/>
+    <tableColumn id="31" xr3:uid="{7791EA87-EAFC-4D2D-8036-CF6616A55DDB}" name="US Core Inflation" dataDxfId="12"/>
+    <tableColumn id="32" xr3:uid="{84A946B2-BC3D-4910-A0B8-DBC39C164652}" name="US Unemployment" dataDxfId="11"/>
+    <tableColumn id="33" xr3:uid="{95419E23-D2CF-4363-BBB2-F3CF2AF2B5EF}" name="US Manufacturing PMI" dataDxfId="10"/>
+    <tableColumn id="34" xr3:uid="{227E5F86-CFBB-4C03-BEF4-03EF7FE57B36}" name="US Services PMI" dataDxfId="9"/>
+    <tableColumn id="35" xr3:uid="{756F9EC1-6A7F-4644-822F-C0FB7871DB43}" name="Eurozone Core Inflation" dataDxfId="8"/>
+    <tableColumn id="36" xr3:uid="{4CC0EE89-317B-47F2-A10D-F3CDBFBD5D1C}" name="Eurozone Unemployment" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06A5E69E-2F40-4D2A-977A-AD36D6E3B9E4}" name="Rho" displayName="Rho" ref="AL1:AL253" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" headerRowBorderDxfId="42" tableBorderDxfId="43" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06A5E69E-2F40-4D2A-977A-AD36D6E3B9E4}" name="Rho" displayName="Rho" ref="AL1:AL253" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{59A2CE30-6406-40C4-8B05-C835995D41AA}" name="Weight" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{59A2CE30-6406-40C4-8B05-C835995D41AA}" name="Weight" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74507980-C7F6-4036-A60E-5A27E2CF363B}" name="Key" displayName="Key" ref="A1:D37" totalsRowShown="0" headerRowDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74507980-C7F6-4036-A60E-5A27E2CF363B}" name="Key" displayName="Key" ref="A1:D37" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:D37" xr:uid="{AC4227FE-A2F0-4FEA-8E2E-5269B0D5A865}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3732D3DF-9E4D-43AB-B48F-AF395AF10F1D}" name="Series"/>
@@ -1896,41 +1894,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF92571-C8FA-4993-8EF6-2CFE52B24ECF}">
   <dimension ref="A1:AL253"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AJ1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="19.125" customWidth="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="20.75" customWidth="1"/>
-    <col min="7" max="7" width="24.625" customWidth="1"/>
-    <col min="8" max="8" width="21.25" customWidth="1"/>
-    <col min="9" max="9" width="38.875" customWidth="1"/>
-    <col min="10" max="10" width="36.75" customWidth="1"/>
-    <col min="11" max="11" width="20.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="13" width="21.125" customWidth="1"/>
-    <col min="14" max="18" width="15.25" customWidth="1"/>
-    <col min="19" max="23" width="16.25" customWidth="1"/>
-    <col min="24" max="24" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="9" max="9" width="38.83203125" customWidth="1"/>
+    <col min="10" max="10" width="36.6640625" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" customWidth="1"/>
+    <col min="14" max="18" width="15.1640625" customWidth="1"/>
+    <col min="19" max="23" width="16.1640625" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" customWidth="1"/>
     <col min="25" max="25" width="26" customWidth="1"/>
-    <col min="26" max="26" width="39.75" customWidth="1"/>
-    <col min="27" max="27" width="16.875" customWidth="1"/>
-    <col min="28" max="28" width="22.875" customWidth="1"/>
-    <col min="29" max="29" width="24.875" customWidth="1"/>
+    <col min="26" max="26" width="39.6640625" customWidth="1"/>
+    <col min="27" max="27" width="16.83203125" customWidth="1"/>
+    <col min="28" max="28" width="22.83203125" customWidth="1"/>
+    <col min="29" max="29" width="24.83203125" customWidth="1"/>
     <col min="30" max="30" width="31.5" customWidth="1"/>
-    <col min="31" max="31" width="17.875" customWidth="1"/>
+    <col min="31" max="31" width="17.83203125" customWidth="1"/>
     <col min="32" max="32" width="19" customWidth="1"/>
     <col min="33" max="33" width="22.5" customWidth="1"/>
-    <col min="34" max="34" width="17.625" customWidth="1"/>
-    <col min="35" max="35" width="23.875" customWidth="1"/>
+    <col min="34" max="34" width="17.6640625" customWidth="1"/>
+    <col min="35" max="35" width="23.83203125" customWidth="1"/>
     <col min="36" max="36" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A2" s="10">
         <v>3.7064468876043577</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A3" s="10">
         <v>-0.51431892706786186</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>5.3028815269757104</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>-2.2338751040316964</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>3.0327192070979834</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>0.58733938392308005</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>4.4694901190888743</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>-0.16160134227196465</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>1.8524117099202613</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
         <v>5.6911606332134284</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
         <v>2.8339206872861809</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>0.20221161992239445</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>2.1666908038923793</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
         <v>9.6901874484194934</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>-1.812131140810763</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
         <v>-1.4508855762338442</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A18" s="10">
         <v>4.7173888865691822</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
         <v>0.42670047789698629</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>1.9716436157610531</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
         <v>2.9770179397713434</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A22" s="10">
         <v>11.479771053572961</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
         <v>-13.540083970359063</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>-7.5180710532073931</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A25" s="10">
         <v>-3.1779582235813564E-2</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A26" s="10">
         <v>1.7199515236815159</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A27" s="10">
         <v>3.6875685916361221</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A28" s="10">
         <v>0.40545816864762685</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A29" s="10">
         <v>2.8817466438326704</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A30" s="10">
         <v>-1.5379034443709685</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A31" s="10">
         <v>2.9825572935635876</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A32" s="10">
         <v>4.6373641445109257</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A33" s="10">
         <v>-5.5445179339539123</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A34" s="10">
         <v>3.4056267086827603</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A35" s="10">
         <v>2.6358002500463016</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A36" s="10">
         <v>3.3718161104984148</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A37" s="10">
         <v>8.0759350919580299</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A38" s="10">
         <v>-8.260552882180022</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A39" s="10">
         <v>1.4185455138679259</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A40" s="10">
         <v>-5.1045441467679353</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A41" s="10">
         <v>0.41492708907347264</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A42" s="10">
         <v>1.5612736622740329</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A43" s="10">
         <v>2.9532925331606776</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A44" s="10">
         <v>-0.46711124048444219</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A45" s="10">
         <v>3.4226595989204043</v>
       </c>
@@ -7059,7 +7059,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A46" s="10">
         <v>3.0118878045340551</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A47" s="10">
         <v>-3.171644634758735</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A48" s="10">
         <v>-2.4743726186334385</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A49" s="10">
         <v>2.161653555943289</v>
       </c>
@@ -7515,7 +7515,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A50" s="10">
         <v>0.75900771040917903</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A51" s="10">
         <v>-0.27382988679067921</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A52" s="10">
         <v>3.5468653928584217</v>
       </c>
@@ -7857,7 +7857,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A53" s="10">
         <v>2.7633511619934836</v>
       </c>
@@ -7971,7 +7971,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A54" s="10">
         <v>-0.19079815823688762</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A55" s="10">
         <v>-0.81480381339484609</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A56" s="10">
         <v>-1.1462839621760992</v>
       </c>
@@ -8313,7 +8313,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A57" s="10">
         <v>-0.96461258414301199</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A58" s="10">
         <v>-0.70596883466036786</v>
       </c>
@@ -8541,7 +8541,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A59" s="10">
         <v>0.49842707660955909</v>
       </c>
@@ -8655,7 +8655,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A60" s="10">
         <v>4.9668756118180966</v>
       </c>
@@ -8769,7 +8769,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A61" s="10">
         <v>5.6017281878965264E-2</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A62" s="10">
         <v>2.8601143888048171</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A63" s="10">
         <v>4.4921776240558273</v>
       </c>
@@ -9111,7 +9111,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A64" s="10">
         <v>0.57693368596156347</v>
       </c>
@@ -9225,7 +9225,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A65" s="10">
         <v>-7.9439651626998398E-2</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A66" s="10">
         <v>0.48340537117223903</v>
       </c>
@@ -9453,7 +9453,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A67" s="10">
         <v>3.6740871522302996</v>
       </c>
@@ -9567,7 +9567,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A68" s="10">
         <v>-0.37531568521519887</v>
       </c>
@@ -9681,7 +9681,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A69" s="10">
         <v>2.9974493834321407</v>
       </c>
@@ -9795,7 +9795,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A70" s="10">
         <v>0.84476311802517046</v>
       </c>
@@ -9909,7 +9909,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A71" s="10">
         <v>2.6300363564941449</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A72" s="10">
         <v>-1.0715217609941448</v>
       </c>
@@ -10137,7 +10137,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A73" s="10">
         <v>-5.7658206514976769</v>
       </c>
@@ -10251,7 +10251,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A74" s="10">
         <v>-4.4878664182658525</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A75" s="10">
         <v>3.3144916933022017</v>
       </c>
@@ -10479,7 +10479,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A76" s="10">
         <v>9.5259645520931855</v>
       </c>
@@ -10593,7 +10593,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A77" s="10">
         <v>-3.3302936416543503</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A78" s="10">
         <v>-8.7434694453718578</v>
       </c>
@@ -10821,7 +10821,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A79" s="10">
         <v>2.364713757350188</v>
       </c>
@@ -10935,7 +10935,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A80" s="10">
         <v>-3.7610690592871663</v>
       </c>
@@ -11049,7 +11049,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A81" s="10">
         <v>2.0325736304644266</v>
       </c>
@@ -11163,7 +11163,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A82" s="10">
         <v>-1.6168280811280908</v>
       </c>
@@ -11277,7 +11277,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A83" s="10">
         <v>2.7145147700443886</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A84" s="10">
         <v>6.4611738870388393</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A85" s="10">
         <v>5.4765720080206961</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A86" s="10">
         <v>0.9347106293041918</v>
       </c>
@@ -11733,7 +11733,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A87" s="10">
         <v>2.2724406087434801</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A88" s="10">
         <v>1.5552067661460285</v>
       </c>
@@ -11961,7 +11961,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A89" s="10">
         <v>0.5967772578233479</v>
       </c>
@@ -12075,7 +12075,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A90" s="10">
         <v>4.2146767463183181</v>
       </c>
@@ -12189,7 +12189,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A91" s="10">
         <v>1.0158581918837939</v>
       </c>
@@ -12303,7 +12303,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A92" s="10">
         <v>1.4575569311049605</v>
       </c>
@@ -12417,7 +12417,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A93" s="10">
         <v>3.8651309870155899</v>
       </c>
@@ -12531,7 +12531,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A94" s="10">
         <v>0.23743791054637597</v>
       </c>
@@ -12645,7 +12645,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A95" s="10">
         <v>0.68534964103257323</v>
       </c>
@@ -12759,7 +12759,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A96" s="10">
         <v>2.4335058864590025</v>
       </c>
@@ -12873,7 +12873,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A97" s="10">
         <v>-2.1700968720873846</v>
       </c>
@@ -12987,7 +12987,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A98" s="10">
         <v>0.60010504313142121</v>
       </c>
@@ -13101,7 +13101,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A99" s="10">
         <v>1.3611143989303685</v>
       </c>
@@ -13215,7 +13215,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A100" s="10">
         <v>3.582730475350786</v>
       </c>
@@ -13329,7 +13329,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A101" s="10">
         <v>2.797046527615322</v>
       </c>
@@ -13443,7 +13443,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A102" s="10">
         <v>-1.495236414391016</v>
       </c>
@@ -13557,7 +13557,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A103" s="10">
         <v>2.4908150349829157</v>
       </c>
@@ -13671,7 +13671,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A104" s="10">
         <v>-3.0850515329939441</v>
       </c>
@@ -13785,7 +13785,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A105" s="10">
         <v>1.1056299123102633</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A106" s="10">
         <v>0.12751042867868989</v>
       </c>
@@ -14013,7 +14013,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A107" s="10">
         <v>3.7196082223705815</v>
       </c>
@@ -14127,7 +14127,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A108" s="10">
         <v>3.9843668591878156</v>
       </c>
@@ -14241,7 +14241,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A109" s="10">
         <v>1.6326387650727554</v>
       </c>
@@ -14355,7 +14355,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A110" s="10">
         <v>0.65703548579286064</v>
       </c>
@@ -14469,7 +14469,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A111" s="10">
         <v>1.0759426602660511</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A112" s="10">
         <v>-1.4295263181476514</v>
       </c>
@@ -14697,7 +14697,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A113" s="10">
         <v>0.89211124201501946</v>
       </c>
@@ -14811,7 +14811,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A114" s="10">
         <v>-5.6511402551535639E-2</v>
       </c>
@@ -14925,7 +14925,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A115" s="10">
         <v>4.3627459369717485</v>
       </c>
@@ -15039,7 +15039,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A116" s="10">
         <v>2.4355394403384594</v>
       </c>
@@ -15153,7 +15153,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A117" s="10">
         <v>-2.5334168892980529</v>
       </c>
@@ -15267,7 +15267,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A118" s="10">
         <v>-0.36416827989084766</v>
       </c>
@@ -15381,7 +15381,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A119" s="10">
         <v>0.52340898184795037</v>
       </c>
@@ -15495,7 +15495,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A120" s="10">
         <v>3.1331032163118806</v>
       </c>
@@ -15609,7 +15609,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A121" s="10">
         <v>4.8190367369414133</v>
       </c>
@@ -15723,7 +15723,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A122" s="10">
         <v>3.5380837547933197</v>
       </c>
@@ -15837,7 +15837,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A123" s="10">
         <v>-2.4985259547676719E-2</v>
       </c>
@@ -15951,7 +15951,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A124" s="10">
         <v>6.9522480870037811</v>
       </c>
@@ -16065,7 +16065,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A125" s="10">
         <v>-2.8005790609298487</v>
       </c>
@@ -16179,7 +16179,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A126" s="10">
         <v>-7.1137336242098996</v>
       </c>
@@ -16293,7 +16293,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A127" s="10">
         <v>-0.92103427262523496</v>
       </c>
@@ -16407,7 +16407,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A128" s="10">
         <v>-2.2910610537168736</v>
       </c>
@@ -16521,7 +16521,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A129" s="10">
         <v>0.64465905240953703</v>
       </c>
@@ -16635,7 +16635,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A130" s="10">
         <v>-0.47310060208863547</v>
       </c>
@@ -16749,7 +16749,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A131" s="10">
         <v>-2.5883640511482326</v>
       </c>
@@ -16863,7 +16863,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A132" s="10">
         <v>2.0828034950095713</v>
       </c>
@@ -16977,7 +16977,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A133" s="10">
         <v>-0.72994832837439105</v>
       </c>
@@ -17091,7 +17091,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A134" s="10">
         <v>4.1091443583711964</v>
       </c>
@@ -17205,7 +17205,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A135" s="10">
         <v>5.0307390801772556</v>
       </c>
@@ -17319,7 +17319,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A136" s="10">
         <v>1.2855798198523161</v>
       </c>
@@ -17433,7 +17433,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A137" s="10">
         <v>1.9067931195030354</v>
       </c>
@@ -17547,7 +17547,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A138" s="10">
         <v>-0.6681068769821934</v>
       </c>
@@ -17661,7 +17661,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A139" s="10">
         <v>1.3955110731164382</v>
       </c>
@@ -17775,7 +17775,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A140" s="10">
         <v>-2.5483050964018048</v>
       </c>
@@ -17889,7 +17889,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A141" s="10">
         <v>-2.2135603150289143</v>
       </c>
@@ -18003,7 +18003,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A142" s="10">
         <v>1.8030822505338051</v>
       </c>
@@ -18117,7 +18117,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A143" s="10">
         <v>7.3867964794934267</v>
       </c>
@@ -18231,7 +18231,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A144" s="10">
         <v>2.9957879358282469</v>
       </c>
@@ -18345,7 +18345,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A145" s="10">
         <v>-1.1648089670725312</v>
       </c>
@@ -18459,7 +18459,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A146" s="10">
         <v>6.9485961381925705</v>
       </c>
@@ -18573,7 +18573,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A147" s="10">
         <v>2.1319217663330789</v>
       </c>
@@ -18687,7 +18687,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A148" s="10">
         <v>-2.0771953606335103</v>
       </c>
@@ -18801,7 +18801,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A149" s="10">
         <v>2.4035380448252539</v>
       </c>
@@ -18915,7 +18915,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A150" s="10">
         <v>3.0134036601175751</v>
       </c>
@@ -19029,7 +19029,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A151" s="10">
         <v>7.0928958038229695</v>
       </c>
@@ -19143,7 +19143,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A152" s="10">
         <v>0.33115769556846431</v>
       </c>
@@ -19257,7 +19257,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A153" s="10">
         <v>2.7505661089179085</v>
       </c>
@@ -19371,7 +19371,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A154" s="10">
         <v>11.98552576641319</v>
       </c>
@@ -19485,7 +19485,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A155" s="10">
         <v>3.4803724971895775</v>
       </c>
@@ -19599,7 +19599,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A156" s="10">
         <v>-8.7676810227813888</v>
       </c>
@@ -19713,7 +19713,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A157" s="10">
         <v>-0.27010546958197779</v>
       </c>
@@ -19827,7 +19827,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A158" s="10">
         <v>-5.8684827671454514</v>
       </c>
@@ -19941,7 +19941,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A159" s="10">
         <v>-6.3132435749313913</v>
       </c>
@@ -20055,7 +20055,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A160" s="10">
         <v>-11.212992009496219</v>
       </c>
@@ -20169,7 +20169,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A161" s="10">
         <v>-8.8846255678260775</v>
       </c>
@@ -20283,7 +20283,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A162" s="10">
         <v>4.0453555777032904</v>
       </c>
@@ -20397,7 +20397,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A163" s="10">
         <v>-1.6529516678750014</v>
       </c>
@@ -20511,7 +20511,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A164" s="10">
         <v>-9.3815630793899913</v>
       </c>
@@ -20625,7 +20625,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A165" s="10">
         <v>2.0075662135618586</v>
       </c>
@@ -20739,7 +20739,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A166" s="10">
         <v>6.7021468615801041</v>
       </c>
@@ -20853,7 +20853,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A167" s="10">
         <v>-5.2674877163427567</v>
       </c>
@@ -20967,7 +20967,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A168" s="10">
         <v>-1.8220176537861619</v>
       </c>
@@ -21081,7 +21081,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A169" s="10">
         <v>-9.8660735078393031</v>
       </c>
@@ -21195,7 +21195,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A170" s="10">
         <v>-0.8093383171472226</v>
       </c>
@@ -21309,7 +21309,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A171" s="10">
         <v>-5.3756196363706295</v>
       </c>
@@ -21423,7 +21423,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A172" s="10">
         <v>2.3253284539505898</v>
       </c>
@@ -21537,7 +21537,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A173" s="10">
         <v>0.65988431600361253</v>
       </c>
@@ -21651,7 +21651,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A174" s="10">
         <v>0.11771178066517507</v>
       </c>
@@ -21765,7 +21765,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A175" s="10">
         <v>-2.5573020381423248</v>
       </c>
@@ -21879,7 +21879,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A176" s="10">
         <v>-0.93977281023522607</v>
       </c>
@@ -21993,7 +21993,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A177" s="10">
         <v>4.4637809590950326</v>
       </c>
@@ -22107,7 +22107,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A178" s="10">
         <v>2.192267712119488</v>
       </c>
@@ -22221,7 +22221,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A179" s="10">
         <v>1.0511492078443467</v>
       </c>
@@ -22335,7 +22335,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A180" s="10">
         <v>-2.0049892103987048</v>
       </c>
@@ -22449,7 +22449,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="181" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A181" s="10">
         <v>2.2720449938202592</v>
       </c>
@@ -22563,7 +22563,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A182" s="10">
         <v>2.5768136560445214</v>
       </c>
@@ -22677,7 +22677,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A183" s="10">
         <v>-0.90269487818478922</v>
       </c>
@@ -22791,7 +22791,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="184" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A184" s="10">
         <v>3.0413678175282399</v>
       </c>
@@ -22905,7 +22905,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A185" s="10">
         <v>2.276540799663735</v>
       </c>
@@ -23019,7 +23019,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A186" s="10">
         <v>2.2202742565758484</v>
       </c>
@@ -23133,7 +23133,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A187" s="10">
         <v>0.87342125896662992</v>
       </c>
@@ -23247,7 +23247,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A188" s="10">
         <v>9.9625364942767192E-2</v>
       </c>
@@ -23361,7 +23361,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A189" s="10">
         <v>-5.253473628794751</v>
       </c>
@@ -23475,7 +23475,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A190" s="10">
         <v>-0.89900183384671095</v>
       </c>
@@ -23589,7 +23589,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A191" s="10">
         <v>0.44390515239696526</v>
       </c>
@@ -23703,7 +23703,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A192" s="10">
         <v>1.8201056286616222</v>
       </c>
@@ -23817,7 +23817,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="193" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A193" s="10">
         <v>2.2770277060045601</v>
       </c>
@@ -23931,7 +23931,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A194" s="10">
         <v>1.9346512430623193</v>
       </c>
@@ -24045,7 +24045,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="195" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A195" s="10">
         <v>5.4281693426455604</v>
       </c>
@@ -24159,7 +24159,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A196" s="10">
         <v>-2.412560201501492</v>
       </c>
@@ -24273,7 +24273,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A197" s="10">
         <v>5.7495125452493738</v>
       </c>
@@ -24387,7 +24387,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A198" s="10">
         <v>-1.059809424652741</v>
       </c>
@@ -24501,7 +24501,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A199" s="10">
         <v>3.5629439216977374</v>
       </c>
@@ -24615,7 +24615,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A200" s="10">
         <v>2.6449176237694587</v>
       </c>
@@ -24729,7 +24729,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="201" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A201" s="10">
         <v>6.5804008635825397</v>
       </c>
@@ -24843,7 +24843,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="202" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A202" s="10">
         <v>-1.514140169923806</v>
       </c>
@@ -24957,7 +24957,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A203" s="10">
         <v>-0.21262025945772223</v>
       </c>
@@ -25071,7 +25071,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="204" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A204" s="10">
         <v>1.9865213053337669</v>
       </c>
@@ -25185,7 +25185,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A205" s="10">
         <v>1.748800204248198</v>
       </c>
@@ -25299,7 +25299,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="206" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A206" s="10">
         <v>1.7635703982167996</v>
       </c>
@@ -25413,7 +25413,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A207" s="10">
         <v>1.6264325394608363</v>
       </c>
@@ -25527,7 +25527,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="208" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A208" s="10">
         <v>-0.45751297033153548</v>
       </c>
@@ -25641,7 +25641,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="209" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A209" s="10">
         <v>8.1011729467803661E-3</v>
       </c>
@@ -25755,7 +25755,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="210" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A210" s="10">
         <v>-0.74711372841854029</v>
       </c>
@@ -25869,7 +25869,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="211" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A211" s="10">
         <v>-1.7481422029282783</v>
       </c>
@@ -25983,7 +25983,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A212" s="10">
         <v>1.8831234724941766</v>
       </c>
@@ -26097,7 +26097,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="213" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A213" s="10">
         <v>-0.94011322161840383</v>
       </c>
@@ -26211,7 +26211,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="214" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A214" s="10">
         <v>0.39002155028866525</v>
       </c>
@@ -26325,7 +26325,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="215" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A215" s="10">
         <v>0.85306381724006997</v>
       </c>
@@ -26439,7 +26439,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="216" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A216" s="10">
         <v>1.6908054983486522</v>
       </c>
@@ -26553,7 +26553,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="217" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A217" s="10">
         <v>2.6426028467643476</v>
       </c>
@@ -26667,7 +26667,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="218" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A218" s="10">
         <v>1.2465040367540752</v>
       </c>
@@ -26781,7 +26781,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="219" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A219" s="10">
         <v>-1.9089815723764332</v>
       </c>
@@ -26895,7 +26895,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="220" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A220" s="10">
         <v>6.6230290301296293</v>
       </c>
@@ -27009,7 +27009,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="221" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A221" s="10">
         <v>-5.198583308496552</v>
       </c>
@@ -27123,7 +27123,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="222" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A222" s="10">
         <v>4.6516921431350085</v>
       </c>
@@ -27237,7 +27237,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="223" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A223" s="10">
         <v>4.7266093080046829</v>
       </c>
@@ -27351,7 +27351,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="224" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A224" s="10">
         <v>4.2891562592263881</v>
       </c>
@@ -27465,7 +27465,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="225" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A225" s="10">
         <v>0.35691844758993341</v>
       </c>
@@ -27579,7 +27579,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="226" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A226" s="10">
         <v>6.2499261391406833</v>
       </c>
@@ -27693,7 +27693,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="227" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A227" s="10">
         <v>-1.4196774181624079</v>
       </c>
@@ -27807,7 +27807,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="228" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A228" s="10">
         <v>-2.152620045137084</v>
       </c>
@@ -27921,7 +27921,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="229" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A229" s="10">
         <v>-5.4310591314182091</v>
       </c>
@@ -28035,7 +28035,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A230" s="10">
         <v>-9.7700782398810588</v>
       </c>
@@ -28149,7 +28149,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="231" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A231" s="10">
         <v>5.0101435644196641</v>
       </c>
@@ -28263,7 +28263,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="232" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A232" s="10">
         <v>6.9296639555078627</v>
       </c>
@@ -28377,7 +28377,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="233" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A233" s="10">
         <v>-11.393404854377849</v>
       </c>
@@ -28491,7 +28491,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A234" s="10">
         <v>-0.25212284442447697</v>
       </c>
@@ -28605,7 +28605,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="235" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A235" s="10">
         <v>-7.1080965082500995</v>
       </c>
@@ -28719,7 +28719,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A236" s="10">
         <v>-11.559261913975007</v>
       </c>
@@ -28833,7 +28833,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="237" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A237" s="10">
         <v>-3.5366350055231521</v>
       </c>
@@ -28947,7 +28947,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A238" s="10">
         <v>-6.3034885396160405</v>
       </c>
@@ -29061,7 +29061,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="239" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A239" s="10">
         <v>4.2012090345409518</v>
       </c>
@@ -29175,7 +29175,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="240" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A240" s="10">
         <v>-1.9023891908141906</v>
       </c>
@@ -29289,7 +29289,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="241" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A241" s="10">
         <v>0.64899274017015784</v>
       </c>
@@ -29403,7 +29403,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="242" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A242" s="10">
         <v>1.6981488841981758</v>
       </c>
@@ -29517,7 +29517,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="243" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A243" s="10">
         <v>6.6075752110920547</v>
       </c>
@@ -29631,7 +29631,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="244" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A244" s="10">
         <v>3.3368748479736752</v>
       </c>
@@ -29745,7 +29745,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="245" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A245" s="10">
         <v>-9.0626301192599783</v>
       </c>
@@ -29859,7 +29859,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="246" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A246" s="10">
         <v>-8.3880887465550842</v>
       </c>
@@ -29973,7 +29973,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="247" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A247" s="10">
         <v>-4.6676947629548806</v>
       </c>
@@ -30087,7 +30087,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="248" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A248" s="10">
         <v>-3.5166611107407135</v>
       </c>
@@ -30201,7 +30201,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="249" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A249" s="10">
         <v>3.9487766540880216</v>
       </c>
@@ -30315,7 +30315,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="250" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A250" s="10">
         <v>5.7370925079425206</v>
       </c>
@@ -30429,7 +30429,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="251" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A251" s="10">
         <v>-1.7769515390628214</v>
       </c>
@@ -30543,7 +30543,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="252" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A252" s="10">
         <v>-7.1395436645017298</v>
       </c>
@@ -30657,7 +30657,7 @@
         <v>3.968253968253968E-3</v>
       </c>
     </row>
-    <row r="253" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A253" s="10">
         <v>3.1776393337604105</v>
       </c>
@@ -30784,17 +30784,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A557845-7B97-49DA-9E9C-9E1E004351D8}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="35.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>87</v>
       </c>
@@ -30808,7 +30810,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -30822,7 +30824,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -30836,7 +30838,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -30850,7 +30852,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -30864,7 +30866,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -30878,7 +30880,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -30892,7 +30894,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -30906,7 +30908,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -30920,7 +30922,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -30934,7 +30936,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -30948,7 +30950,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -30962,7 +30964,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -30976,7 +30978,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
@@ -30990,7 +30992,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -31004,7 +31006,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -31018,7 +31020,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -31032,7 +31034,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -31046,7 +31048,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -31060,7 +31062,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -31074,7 +31076,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -31088,7 +31090,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -31102,7 +31104,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -31116,7 +31118,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -31130,7 +31132,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -31144,7 +31146,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -31158,7 +31160,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -31172,7 +31174,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -31186,7 +31188,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -31200,7 +31202,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -31214,7 +31216,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -31228,7 +31230,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -31242,7 +31244,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -31256,7 +31258,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -31270,7 +31272,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -31284,7 +31286,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -31298,7 +31300,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -31324,17 +31326,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A23E9E-AD58-405A-B1C1-3611BDB303BD}">
   <dimension ref="A1:D252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -31347,7 +31349,7 @@
         <v>3.7064468876043577</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -31360,14 +31362,14 @@
         <v>-0.51431892706786186</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B3" s="7"/>
       <c r="D3" s="4">
         <f ca="1"/>
         <v>5.3028815269757104</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -31379,7 +31381,7 @@
         <v>-2.2338751040316964</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -31392,7 +31394,7 @@
         <v>3.0327192070979834</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -31405,7 +31407,7 @@
         <v>0.58733938392308005</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -31418,1471 +31420,1471 @@
         <v>4.4694901190888743</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D8" s="4">
         <f ca="1"/>
         <v>-0.16160134227196465</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D9" s="4">
         <f ca="1"/>
         <v>1.8524117099202613</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D10" s="4">
         <f ca="1"/>
         <v>5.6911606332134284</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D11" s="4">
         <f ca="1"/>
         <v>2.8339206872861809</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D12" s="4">
         <f ca="1"/>
         <v>0.20221161992239445</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D13" s="4">
         <f ca="1"/>
         <v>2.1666908038923793</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D14" s="4">
         <f ca="1"/>
         <v>9.6901874484194934</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D15" s="4">
         <f ca="1"/>
         <v>-1.812131140810763</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D16" s="4">
         <f ca="1"/>
         <v>-1.4508855762338442</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D17" s="4">
         <f ca="1"/>
         <v>4.7173888865691822</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D18" s="4">
         <f ca="1"/>
         <v>0.42670047789698629</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D19" s="4">
         <f ca="1"/>
         <v>1.9716436157610531</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D20" s="4">
         <f ca="1"/>
         <v>2.9770179397713434</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D21" s="4">
         <f ca="1"/>
         <v>11.479771053572961</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D22" s="4">
         <f ca="1"/>
         <v>-13.540083970359063</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D23" s="4">
         <f ca="1"/>
         <v>-7.5180710532073931</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D24" s="4">
         <f ca="1"/>
         <v>-3.1779582235813564E-2</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D25" s="4">
         <f ca="1"/>
         <v>1.7199515236815159</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D26" s="4">
         <f ca="1"/>
         <v>3.6875685916361221</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D27" s="4">
         <f ca="1"/>
         <v>0.40545816864762685</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D28" s="4">
         <f ca="1"/>
         <v>2.8817466438326704</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D29" s="4">
         <f ca="1"/>
         <v>-1.5379034443709685</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D30" s="4">
         <f ca="1"/>
         <v>2.9825572935635876</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D31" s="4">
         <f ca="1"/>
         <v>4.6373641445109257</v>
       </c>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D32" s="4">
         <f ca="1"/>
         <v>-5.5445179339539123</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D33" s="4">
         <f ca="1"/>
         <v>3.4056267086827603</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D34" s="4">
         <f ca="1"/>
         <v>2.6358002500463016</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D35" s="4">
         <f ca="1"/>
         <v>3.3718161104984148</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D36" s="4">
         <f ca="1"/>
         <v>8.0759350919580299</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D37" s="4">
         <f ca="1"/>
         <v>-8.260552882180022</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D38" s="4">
         <f ca="1"/>
         <v>1.4185455138679259</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D39" s="4">
         <f ca="1"/>
         <v>-5.1045441467679353</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D40" s="4">
         <f ca="1"/>
         <v>0.41492708907347264</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D41" s="4">
         <f ca="1"/>
         <v>1.5612736622740329</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D42" s="4">
         <f ca="1"/>
         <v>2.9532925331606776</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D43" s="4">
         <f ca="1"/>
         <v>-0.46711124048444219</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D44" s="4">
         <f ca="1"/>
         <v>3.4226595989204043</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D45" s="4">
         <f ca="1"/>
         <v>3.0118878045340551</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D46" s="4">
         <f ca="1"/>
         <v>-3.171644634758735</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D47" s="4">
         <f ca="1"/>
         <v>-2.4743726186334385</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D48" s="4">
         <f ca="1"/>
         <v>2.161653555943289</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D49" s="4">
         <f ca="1"/>
         <v>0.75900771040917903</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D50" s="4">
         <f ca="1"/>
         <v>-0.27382988679067921</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D51" s="4">
         <f ca="1"/>
         <v>3.5468653928584217</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D52" s="4">
         <f ca="1"/>
         <v>2.7633511619934836</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D53" s="4">
         <f ca="1"/>
         <v>-0.19079815823688762</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D54" s="4">
         <f ca="1"/>
         <v>-0.81480381339484609</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D55" s="4">
         <f ca="1"/>
         <v>-1.1462839621760992</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D56" s="4">
         <f ca="1"/>
         <v>-0.96461258414301199</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D57" s="4">
         <f ca="1"/>
         <v>-0.70596883466036786</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D58" s="4">
         <f ca="1"/>
         <v>0.49842707660955909</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D59" s="4">
         <f ca="1"/>
         <v>4.9668756118180966</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D60" s="4">
         <f ca="1"/>
         <v>5.6017281878965264E-2</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D61" s="4">
         <f ca="1"/>
         <v>2.8601143888048171</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D62" s="4">
         <f ca="1"/>
         <v>4.4921776240558273</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D63" s="4">
         <f ca="1"/>
         <v>0.57693368596156347</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D64" s="4">
         <f ca="1"/>
         <v>-7.9439651626998398E-2</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D65" s="4">
         <f ca="1"/>
         <v>0.48340537117223903</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D66" s="4">
         <f ca="1"/>
         <v>3.6740871522302996</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D67" s="4">
         <f ca="1"/>
         <v>-0.37531568521519887</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D68" s="4">
         <f ca="1"/>
         <v>2.9974493834321407</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D69" s="4">
         <f ca="1"/>
         <v>0.84476311802517046</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D70" s="4">
         <f ca="1"/>
         <v>2.6300363564941449</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D71" s="4">
         <f ca="1"/>
         <v>-1.0715217609941448</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D72" s="4">
         <f ca="1"/>
         <v>-5.7658206514976769</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D73" s="4">
         <f ca="1"/>
         <v>-4.4878664182658525</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D74" s="4">
         <f ca="1"/>
         <v>3.3144916933022017</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D75" s="4">
         <f ca="1"/>
         <v>9.5259645520931855</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D76" s="4">
         <f ca="1"/>
         <v>-3.3302936416543503</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D77" s="4">
         <f ca="1"/>
         <v>-8.7434694453718578</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D78" s="4">
         <f ca="1"/>
         <v>2.364713757350188</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D79" s="4">
         <f ca="1"/>
         <v>-3.7610690592871663</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D80" s="4">
         <f ca="1"/>
         <v>2.0325736304644266</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D81" s="4">
         <f ca="1"/>
         <v>-1.6168280811280908</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D82" s="4">
         <f ca="1"/>
         <v>2.7145147700443886</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D83" s="4">
         <f ca="1"/>
         <v>6.4611738870388393</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D84" s="4">
         <f ca="1"/>
         <v>5.4765720080206961</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D85" s="4">
         <f ca="1"/>
         <v>0.9347106293041918</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D86" s="4">
         <f ca="1"/>
         <v>2.2724406087434801</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D87" s="4">
         <f ca="1"/>
         <v>1.5552067661460285</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D88" s="4">
         <f ca="1"/>
         <v>0.5967772578233479</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D89" s="4">
         <f ca="1"/>
         <v>4.2146767463183181</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D90" s="4">
         <f ca="1"/>
         <v>1.0158581918837939</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D91" s="4">
         <f ca="1"/>
         <v>1.4575569311049605</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D92" s="4">
         <f ca="1"/>
         <v>3.8651309870155899</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D93" s="4">
         <f ca="1"/>
         <v>0.23743791054637597</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D94" s="4">
         <f ca="1"/>
         <v>0.68534964103257323</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D95" s="4">
         <f ca="1"/>
         <v>2.4335058864590025</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D96" s="4">
         <f ca="1"/>
         <v>-2.1700968720873846</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D97" s="4">
         <f ca="1"/>
         <v>0.60010504313142121</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D98" s="4">
         <f ca="1"/>
         <v>1.3611143989303685</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D99" s="4">
         <f ca="1"/>
         <v>3.582730475350786</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D100" s="4">
         <f ca="1"/>
         <v>2.797046527615322</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D101" s="4">
         <f ca="1"/>
         <v>-1.495236414391016</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D102" s="4">
         <f ca="1"/>
         <v>2.4908150349829157</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D103" s="4">
         <f ca="1"/>
         <v>-3.0850515329939441</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D104" s="4">
         <f ca="1"/>
         <v>1.1056299123102633</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D105" s="4">
         <f ca="1"/>
         <v>0.12751042867868989</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D106" s="4">
         <f ca="1"/>
         <v>3.7196082223705815</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D107" s="4">
         <f ca="1"/>
         <v>3.9843668591878156</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D108" s="4">
         <f ca="1"/>
         <v>1.6326387650727554</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D109" s="4">
         <f ca="1"/>
         <v>0.65703548579286064</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D110" s="4">
         <f ca="1"/>
         <v>1.0759426602660511</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D111" s="4">
         <f ca="1"/>
         <v>-1.4295263181476514</v>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D112" s="4">
         <f ca="1"/>
         <v>0.89211124201501946</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D113" s="4">
         <f ca="1"/>
         <v>-5.6511402551535639E-2</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D114" s="4">
         <f ca="1"/>
         <v>4.3627459369717485</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D115" s="4">
         <f ca="1"/>
         <v>2.4355394403384594</v>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D116" s="4">
         <f ca="1"/>
         <v>-2.5334168892980529</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D117" s="4">
         <f ca="1"/>
         <v>-0.36416827989084766</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D118" s="4">
         <f ca="1"/>
         <v>0.52340898184795037</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D119" s="4">
         <f ca="1"/>
         <v>3.1331032163118806</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D120" s="4">
         <f ca="1"/>
         <v>4.8190367369414133</v>
       </c>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D121" s="4">
         <f ca="1"/>
         <v>3.5380837547933197</v>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D122" s="4">
         <f ca="1"/>
         <v>-2.4985259547676719E-2</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D123" s="4">
         <f ca="1"/>
         <v>6.9522480870037811</v>
       </c>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D124" s="4">
         <f ca="1"/>
         <v>-2.8005790609298487</v>
       </c>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D125" s="4">
         <f ca="1"/>
         <v>-7.1137336242098996</v>
       </c>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D126" s="4">
         <f ca="1"/>
         <v>-0.92103427262523496</v>
       </c>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D127" s="4">
         <f ca="1"/>
         <v>-2.2910610537168736</v>
       </c>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D128" s="4">
         <f ca="1"/>
         <v>0.64465905240953703</v>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D129" s="4">
         <f ca="1"/>
         <v>-0.47310060208863547</v>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D130" s="4">
         <f ca="1"/>
         <v>-2.5883640511482326</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D131" s="4">
         <f ca="1"/>
         <v>2.0828034950095713</v>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D132" s="4">
         <f ca="1"/>
         <v>-0.72994832837439105</v>
       </c>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D133" s="4">
         <f ca="1"/>
         <v>4.1091443583711964</v>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D134" s="4">
         <f ca="1"/>
         <v>5.0307390801772556</v>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D135" s="4">
         <f ca="1"/>
         <v>1.2855798198523161</v>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D136" s="4">
         <f ca="1"/>
         <v>1.9067931195030354</v>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D137" s="4">
         <f ca="1"/>
         <v>-0.6681068769821934</v>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D138" s="4">
         <f ca="1"/>
         <v>1.3955110731164382</v>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D139" s="4">
         <f ca="1"/>
         <v>-2.5483050964018048</v>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D140" s="4">
         <f ca="1"/>
         <v>-2.2135603150289143</v>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D141" s="4">
         <f ca="1"/>
         <v>1.8030822505338051</v>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D142" s="4">
         <f ca="1"/>
         <v>7.3867964794934267</v>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D143" s="4">
         <f ca="1"/>
         <v>2.9957879358282469</v>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D144" s="4">
         <f ca="1"/>
         <v>-1.1648089670725312</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D145" s="4">
         <f ca="1"/>
         <v>6.9485961381925705</v>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D146" s="4">
         <f ca="1"/>
         <v>2.1319217663330789</v>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D147" s="4">
         <f ca="1"/>
         <v>-2.0771953606335103</v>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D148" s="4">
         <f ca="1"/>
         <v>2.4035380448252539</v>
       </c>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D149" s="4">
         <f ca="1"/>
         <v>3.0134036601175751</v>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D150" s="4">
         <f ca="1"/>
         <v>7.0928958038229695</v>
       </c>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D151" s="4">
         <f ca="1"/>
         <v>0.33115769556846431</v>
       </c>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D152" s="4">
         <f ca="1"/>
         <v>2.7505661089179085</v>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D153" s="4">
         <f ca="1"/>
         <v>11.98552576641319</v>
       </c>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D154" s="4">
         <f ca="1"/>
         <v>3.4803724971895775</v>
       </c>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D155" s="4">
         <f ca="1"/>
         <v>-8.7676810227813888</v>
       </c>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D156" s="4">
         <f ca="1"/>
         <v>-0.27010546958197779</v>
       </c>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D157" s="4">
         <f ca="1"/>
         <v>-5.8684827671454514</v>
       </c>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D158" s="4">
         <f ca="1"/>
         <v>-6.3132435749313913</v>
       </c>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D159" s="4">
         <f ca="1"/>
         <v>-11.212992009496219</v>
       </c>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D160" s="4">
         <f ca="1"/>
         <v>-8.8846255678260775</v>
       </c>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D161" s="4">
         <f ca="1"/>
         <v>4.0453555777032904</v>
       </c>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D162" s="4">
         <f ca="1"/>
         <v>-1.6529516678750014</v>
       </c>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D163" s="4">
         <f ca="1"/>
         <v>-9.3815630793899913</v>
       </c>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D164" s="4">
         <f ca="1"/>
         <v>2.0075662135618586</v>
       </c>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D165" s="4">
         <f ca="1"/>
         <v>6.7021468615801041</v>
       </c>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D166" s="4">
         <f ca="1"/>
         <v>-5.2674877163427567</v>
       </c>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D167" s="4">
         <f ca="1"/>
         <v>-1.8220176537861619</v>
       </c>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D168" s="4">
         <f ca="1"/>
         <v>-9.8660735078393031</v>
       </c>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D169" s="4">
         <f ca="1"/>
         <v>-0.8093383171472226</v>
       </c>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D170" s="4">
         <f ca="1"/>
         <v>-5.3756196363706295</v>
       </c>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D171" s="4">
         <f ca="1"/>
         <v>2.3253284539505898</v>
       </c>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D172" s="4">
         <f ca="1"/>
         <v>0.65988431600361253</v>
       </c>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D173" s="4">
         <f ca="1"/>
         <v>0.11771178066517507</v>
       </c>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D174" s="4">
         <f ca="1"/>
         <v>-2.5573020381423248</v>
       </c>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D175" s="4">
         <f ca="1"/>
         <v>-0.93977281023522607</v>
       </c>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D176" s="4">
         <f ca="1"/>
         <v>4.4637809590950326</v>
       </c>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D177" s="4">
         <f ca="1"/>
         <v>2.192267712119488</v>
       </c>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D178" s="4">
         <f ca="1"/>
         <v>1.0511492078443467</v>
       </c>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D179" s="4">
         <f ca="1"/>
         <v>-2.0049892103987048</v>
       </c>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D180" s="4">
         <f ca="1"/>
         <v>2.2720449938202592</v>
       </c>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D181" s="4">
         <f ca="1"/>
         <v>2.5768136560445214</v>
       </c>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D182" s="4">
         <f ca="1"/>
         <v>-0.90269487818478922</v>
       </c>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D183" s="4">
         <f ca="1"/>
         <v>3.0413678175282399</v>
       </c>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D184" s="4">
         <f ca="1"/>
         <v>2.276540799663735</v>
       </c>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D185" s="4">
         <f ca="1"/>
         <v>2.2202742565758484</v>
       </c>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D186" s="4">
         <f ca="1"/>
         <v>0.87342125896662992</v>
       </c>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D187" s="4">
         <f ca="1"/>
         <v>9.9625364942767192E-2</v>
       </c>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D188" s="4">
         <f ca="1"/>
         <v>-5.253473628794751</v>
       </c>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D189" s="4">
         <f ca="1"/>
         <v>-0.89900183384671095</v>
       </c>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D190" s="4">
         <f ca="1"/>
         <v>0.44390515239696526</v>
       </c>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D191" s="4">
         <f ca="1"/>
         <v>1.8201056286616222</v>
       </c>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D192" s="4">
         <f ca="1"/>
         <v>2.2770277060045601</v>
       </c>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D193" s="4">
         <f ca="1"/>
         <v>1.9346512430623193</v>
       </c>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D194" s="4">
         <f ca="1"/>
         <v>5.4281693426455604</v>
       </c>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D195" s="4">
         <f ca="1"/>
         <v>-2.412560201501492</v>
       </c>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D196" s="4">
         <f ca="1"/>
         <v>5.7495125452493738</v>
       </c>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D197" s="4">
         <f ca="1"/>
         <v>-1.059809424652741</v>
       </c>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D198" s="4">
         <f ca="1"/>
         <v>3.5629439216977374</v>
       </c>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D199" s="4">
         <f ca="1"/>
         <v>2.6449176237694587</v>
       </c>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D200" s="4">
         <f ca="1"/>
         <v>6.5804008635825397</v>
       </c>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D201" s="4">
         <f ca="1"/>
         <v>-1.514140169923806</v>
       </c>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D202" s="4">
         <f ca="1"/>
         <v>-0.21262025945772223</v>
       </c>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D203" s="4">
         <f ca="1"/>
         <v>1.9865213053337669</v>
       </c>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D204" s="4">
         <f ca="1"/>
         <v>1.748800204248198</v>
       </c>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D205" s="4">
         <f ca="1"/>
         <v>1.7635703982167996</v>
       </c>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D206" s="4">
         <f ca="1"/>
         <v>1.6264325394608363</v>
       </c>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D207" s="4">
         <f ca="1"/>
         <v>-0.45751297033153548</v>
       </c>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D208" s="4">
         <f ca="1"/>
         <v>8.1011729467803661E-3</v>
       </c>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D209" s="4">
         <f ca="1"/>
         <v>-0.74711372841854029</v>
       </c>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D210" s="4">
         <f ca="1"/>
         <v>-1.7481422029282783</v>
       </c>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D211" s="4">
         <f ca="1"/>
         <v>1.8831234724941766</v>
       </c>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D212" s="4">
         <f ca="1"/>
         <v>-0.94011322161840383</v>
       </c>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D213" s="4">
         <f ca="1"/>
         <v>0.39002155028866525</v>
       </c>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D214" s="4">
         <f ca="1"/>
         <v>0.85306381724006997</v>
       </c>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D215" s="4">
         <f ca="1"/>
         <v>1.6908054983486522</v>
       </c>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D216" s="4">
         <f ca="1"/>
         <v>2.6426028467643476</v>
       </c>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D217" s="4">
         <f ca="1"/>
         <v>1.2465040367540752</v>
       </c>
     </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D218" s="4">
         <f ca="1"/>
         <v>-1.9089815723764332</v>
       </c>
     </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D219" s="4">
         <f ca="1"/>
         <v>6.6230290301296293</v>
       </c>
     </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D220" s="4">
         <f ca="1"/>
         <v>-5.198583308496552</v>
       </c>
     </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D221" s="4">
         <f ca="1"/>
         <v>4.6516921431350085</v>
       </c>
     </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D222" s="4">
         <f ca="1"/>
         <v>4.7266093080046829</v>
       </c>
     </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D223" s="4">
         <f ca="1"/>
         <v>4.2891562592263881</v>
       </c>
     </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D224" s="4">
         <f ca="1"/>
         <v>0.35691844758993341</v>
       </c>
     </row>
-    <row r="225" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D225" s="4">
         <f ca="1"/>
         <v>6.2499261391406833</v>
       </c>
     </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D226" s="4">
         <f ca="1"/>
         <v>-1.4196774181624079</v>
       </c>
     </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D227" s="4">
         <f ca="1"/>
         <v>-2.152620045137084</v>
       </c>
     </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D228" s="4">
         <f ca="1"/>
         <v>-5.4310591314182091</v>
       </c>
     </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D229" s="4">
         <f ca="1"/>
         <v>-9.7700782398810588</v>
       </c>
     </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D230" s="4">
         <f ca="1"/>
         <v>5.0101435644196641</v>
       </c>
     </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D231" s="4">
         <f ca="1"/>
         <v>6.9296639555078627</v>
       </c>
     </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D232" s="4">
         <f ca="1"/>
         <v>-11.393404854377849</v>
       </c>
     </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D233" s="4">
         <f ca="1"/>
         <v>-0.25212284442447697</v>
       </c>
     </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D234" s="4">
         <f ca="1"/>
         <v>-7.1080965082500995</v>
       </c>
     </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D235" s="4">
         <f ca="1"/>
         <v>-11.559261913975007</v>
       </c>
     </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D236" s="4">
         <f ca="1"/>
         <v>-3.5366350055231521</v>
       </c>
     </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D237" s="4">
         <f ca="1"/>
         <v>-6.3034885396160405</v>
       </c>
     </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D238" s="4">
         <f ca="1"/>
         <v>4.2012090345409518</v>
       </c>
     </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D239" s="4">
         <f ca="1"/>
         <v>-1.9023891908141906</v>
       </c>
     </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D240" s="4">
         <f ca="1"/>
         <v>0.64899274017015784</v>
       </c>
     </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D241" s="4">
         <f ca="1"/>
         <v>1.6981488841981758</v>
       </c>
     </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D242" s="4">
         <f ca="1"/>
         <v>6.6075752110920547</v>
       </c>
     </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D243" s="4">
         <f ca="1"/>
         <v>3.3368748479736752</v>
       </c>
     </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D244" s="4">
         <f ca="1"/>
         <v>-9.0626301192599783</v>
       </c>
     </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D245" s="4">
         <f ca="1"/>
         <v>-8.3880887465550842</v>
       </c>
     </row>
-    <row r="246" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D246" s="4">
         <f ca="1"/>
         <v>-4.6676947629548806</v>
       </c>
     </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D247" s="4">
         <f ca="1"/>
         <v>-3.5166611107407135</v>
       </c>
     </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D248" s="4">
         <f ca="1"/>
         <v>3.9487766540880216</v>
       </c>
     </row>
-    <row r="249" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D249" s="4">
         <f ca="1"/>
         <v>5.7370925079425206</v>
       </c>
     </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D250" s="4">
         <f ca="1"/>
         <v>-1.7769515390628214</v>
       </c>
     </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D251" s="4">
         <f ca="1"/>
         <v>-7.1395436645017298</v>
       </c>
     </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D252" s="4">
         <f ca="1"/>
         <v>3.1776393337604105</v>

</xml_diff>